<commit_message>
add new design css addition, additional flags in the scripts, and fix error in createdom.py caused by int and str concat
</commit_message>
<xml_diff>
--- a/assets/headlines.xlsx
+++ b/assets/headlines.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daniel.Wood/Documents/sites/quizzer1/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="4220" windowWidth="25360" windowHeight="18740" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -118,6 +126,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -445,13 +458,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -482,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -496,10 +507,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>